<commit_message>
fix: cambia la tabla sensibilidad
</commit_message>
<xml_diff>
--- a/res/sensibilidad.xlsx
+++ b/res/sensibilidad.xlsx
@@ -386,87 +386,87 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>389725.3899023259</v>
+        <v>264678.4274872866</v>
       </c>
       <c r="B2">
-        <v>321474.3733763354</v>
+        <v>220265.610095929</v>
       </c>
       <c r="C2">
-        <v>266612.7400939023</v>
+        <v>184793.0682734134</v>
       </c>
       <c r="D2">
-        <v>222587.9169773016</v>
+        <v>156431.1092878721</v>
       </c>
       <c r="E2">
-        <v>187272.2952660974</v>
+        <v>133700.69611276</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>473479.9394129804</v>
+        <v>320876.0600554887</v>
       </c>
       <c r="B3">
-        <v>389725.3899023259</v>
+        <v>265652.9572145922</v>
       </c>
       <c r="C3">
-        <v>322062.4270923145</v>
+        <v>221434.3448355638</v>
       </c>
       <c r="D3">
-        <v>267558.0992372333</v>
+        <v>186039.4470370775</v>
       </c>
       <c r="E3">
-        <v>223726.5962144691</v>
+        <v>157679.3479733003</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>574562.0712581592</v>
+        <v>389725.3899023259</v>
       </c>
       <c r="B4">
-        <v>472596.1001033363</v>
+        <v>321474.3733763354</v>
       </c>
       <c r="C4">
-        <v>389725.3899023259</v>
+        <v>266612.7400939023</v>
       </c>
       <c r="D4">
-        <v>322640.481462321</v>
+        <v>222587.9169773016</v>
       </c>
       <c r="E4">
-        <v>268489.3487276214</v>
+        <v>187272.2952660974</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>695522.7270597054</v>
+        <v>473479.9394129804</v>
       </c>
       <c r="B5">
-        <v>572439.0578652468</v>
+        <v>389725.3899023259</v>
       </c>
       <c r="C5">
-        <v>471730.6492735636</v>
+        <v>322062.4270923145</v>
       </c>
       <c r="D5">
-        <v>389725.3899023259</v>
+        <v>267558.0992372333</v>
       </c>
       <c r="E5">
-        <v>323208.7880676879</v>
+        <v>223726.5962144691</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>839001.2406154437</v>
+        <v>574562.0712581592</v>
       </c>
       <c r="B6">
-        <v>691730.9055806599</v>
+        <v>472596.1001033363</v>
       </c>
       <c r="C6">
-        <v>570363.6051451492</v>
+        <v>389725.3899023259</v>
       </c>
       <c r="D6">
-        <v>470883.0209088749</v>
+        <v>322640.481462321</v>
       </c>
       <c r="E6">
-        <v>389725.3899023259</v>
+        <v>268489.3487276214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>